<commit_message>
added timekeeper and measurements
</commit_message>
<xml_diff>
--- a/services/manager/rules.xlsx
+++ b/services/manager/rules.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\MASTER\SERVICES\DISTRIBUTOR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\[SCHULE]\MASTERARBEIT\REPO\wfc_old\services\manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D553189F-86A5-41EE-A51A-EA6A4ED411F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F2292E-0AFE-48B4-96E1-11F900320558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="5520" windowWidth="24225" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="6030" windowWidth="21600" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>numberOfTilesX</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>VALUE</t>
+  </si>
+  <si>
+    <t>numberOfWorkers</t>
   </si>
 </sst>
 </file>
@@ -361,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,6 +415,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>